<commit_message>
local changes jason laptop
</commit_message>
<xml_diff>
--- a/data/supertuxkart-active-passive/metadata/engagement_reseponse_survey_final.xlsx
+++ b/data/supertuxkart-active-passive/metadata/engagement_reseponse_survey_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiseu\stimulus-response-analysis\data\supertuxkart-active-passive\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jiseu\Softwares\Active-Passive-SRC-Publication\data\supertuxkart-active-passive\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907A574D-3857-4725-BCF8-7382E456C7F1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E422B743-F899-4049-92A5-CDD37AE773F4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Timestamp</t>
   </si>
@@ -59,6 +59,60 @@
   </si>
   <si>
     <t>Subject Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alex Gustavo Chalco Maza</t>
+  </si>
+  <si>
+    <t>Usman Arshad</t>
+  </si>
+  <si>
+    <t>Destiny Berisha</t>
+  </si>
+  <si>
+    <t>Nadia Sultana</t>
+  </si>
+  <si>
+    <t>Fahmida Ferdousi</t>
+  </si>
+  <si>
+    <t>Hadia Perez</t>
+  </si>
+  <si>
+    <t>Jung Sang Cho</t>
+  </si>
+  <si>
+    <t>Kevin Call</t>
+  </si>
+  <si>
+    <t>Nicole Vazquez</t>
+  </si>
+  <si>
+    <t>James Castro</t>
+  </si>
+  <si>
+    <t>Jasmine Bachtarzi</t>
+  </si>
+  <si>
+    <t>Jean Carlos Huang</t>
+  </si>
+  <si>
+    <t>Taehyuk Kim</t>
+  </si>
+  <si>
+    <t>Syed Rizvi</t>
+  </si>
+  <si>
+    <t>Revital Schechter</t>
+  </si>
+  <si>
+    <t>Nicholas Carter</t>
+  </si>
+  <si>
+    <t>Aren Mineo</t>
+  </si>
+  <si>
+    <t>Ridmila Sudasinghe</t>
   </si>
 </sst>
 </file>
@@ -474,19 +528,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomLeft" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="11" width="21.5703125" customWidth="1"/>
+    <col min="1" max="11" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -515,7 +569,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>43056.627650462964</v>
       </c>
@@ -541,7 +595,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>43067.736018518517</v>
       </c>
@@ -569,8 +623,11 @@
       <c r="I3" s="7">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>43068.675370370373</v>
       </c>
@@ -598,8 +655,11 @@
       <c r="I4" s="7">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>43068.837187500001</v>
       </c>
@@ -627,8 +687,11 @@
       <c r="I5" s="8">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>43069.744652777779</v>
       </c>
@@ -656,8 +719,11 @@
       <c r="I6" s="8">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>43070.67560185185</v>
       </c>
@@ -685,8 +751,11 @@
       <c r="I7" s="8">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>43070.793402777781</v>
       </c>
@@ -714,8 +783,11 @@
       <c r="I8" s="8">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>43073.894224537034</v>
       </c>
@@ -743,8 +815,11 @@
       <c r="I9" s="8">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>43074.762997685182</v>
       </c>
@@ -772,8 +847,11 @@
       <c r="I10" s="8">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>43075.690567129626</v>
       </c>
@@ -801,8 +879,11 @@
       <c r="I11" s="8">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>43075.786157407405</v>
       </c>
@@ -830,8 +911,11 @@
       <c r="I12" s="8">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>43076.733252314814</v>
       </c>
@@ -859,8 +943,11 @@
       <c r="I13" s="8">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>43082.640659722223</v>
       </c>
@@ -888,8 +975,11 @@
       <c r="I14" s="8">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>43150.738576388889</v>
       </c>
@@ -915,7 +1005,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>43151.550902777781</v>
       </c>
@@ -941,7 +1031,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>43151.77412037037</v>
       </c>
@@ -967,7 +1057,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>43152.545775462961</v>
       </c>
@@ -993,7 +1083,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>43152.708055555559</v>
       </c>
@@ -1019,7 +1109,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>43153.616157407407</v>
       </c>
@@ -1047,8 +1137,11 @@
       <c r="I20" s="8">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>43153.774189814816</v>
       </c>
@@ -1076,8 +1169,11 @@
       <c r="I21" s="8">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>43161.683472222219</v>
       </c>
@@ -1105,8 +1201,11 @@
       <c r="I22" s="8">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>43162.480868055558</v>
       </c>
@@ -1134,8 +1233,11 @@
       <c r="I23" s="8">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>43162.593842592592</v>
       </c>
@@ -1163,8 +1265,11 @@
       <c r="I24" s="8">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>43165.61923611111</v>
       </c>
@@ -1191,6 +1296,9 @@
       </c>
       <c r="I25" s="8">
         <v>22</v>
+      </c>
+      <c r="J25" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1203,13 +1311,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>

</xml_diff>